<commit_message>
More Results figure prep work
</commit_message>
<xml_diff>
--- a/reports/ReportData.xlsx
+++ b/reports/ReportData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t xml:space="preserve">Test Errors by Variable </t>
   </si>
@@ -105,15 +105,6 @@
     <t>Accuracy per Complexity</t>
   </si>
   <si>
-    <t>Baseline LR (train on all cells)</t>
-  </si>
-  <si>
-    <t>Baseline LR (train on single cell)</t>
-  </si>
-  <si>
-    <t>Baseline LR w/ single cell, LASSO</t>
-  </si>
-  <si>
     <t>Non-regularized results</t>
   </si>
   <si>
@@ -126,25 +117,28 @@
     <t>VAR(1) trained on single cell</t>
   </si>
   <si>
-    <t>Baseline LR trained on single cell</t>
-  </si>
-  <si>
     <t>Lasso-regularized Results</t>
   </si>
   <si>
-    <t>Baseline LR w/ all cells, LASSO</t>
-  </si>
-  <si>
     <t>VAR(10) trained on all cells</t>
   </si>
   <si>
-    <t>Baseline LR trained on all cells</t>
-  </si>
-  <si>
     <t>VAR(2) trained on all cells</t>
   </si>
   <si>
     <t>VAR(1) trained on all cells</t>
+  </si>
+  <si>
+    <t>LR trained on all cells</t>
+  </si>
+  <si>
+    <t>LR trained on single cell</t>
+  </si>
+  <si>
+    <t>LR trained on all cells, LASSO</t>
+  </si>
+  <si>
+    <t>LR trained on single cell, LASSO</t>
   </si>
 </sst>
 </file>
@@ -299,7 +293,15 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>RMSE for Single-Cell Models</a:t>
+              <a:t>RMSE for Single</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cell Models</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -512,7 +514,7 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Baseline LR trained on single cell</c:v>
+                  <c:v>LR trained on single cell</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>VAR(1) trained on single cell</c:v>
@@ -575,7 +577,7 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Baseline LR trained on single cell</c:v>
+                  <c:v>LR trained on single cell</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>VAR(1) trained on single cell</c:v>
@@ -657,6 +659,25 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
@@ -941,7 +962,7 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Baseline LR trained on all cells</c:v>
+                  <c:v>LR trained on all cells</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>VAR(1) trained on all cells</c:v>
@@ -1004,7 +1025,7 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Baseline LR trained on all cells</c:v>
+                  <c:v>LR trained on all cells</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>VAR(1) trained on all cells</c:v>
@@ -1086,6 +1107,25 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
@@ -1129,15 +1169,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:colOff>847725</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1158,16 +1198,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1752600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1481,7 +1521,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,12 +1609,12 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B7" s="15">
         <v>0.66499208370129603</v>
@@ -1624,7 +1664,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2">
         <v>0.95244427414566502</v>
@@ -1675,7 +1715,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2">
         <v>1.2007853203182199</v>
@@ -1726,17 +1766,17 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1894,12 +1934,12 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19" s="15">
         <v>0.89801268782257704</v>
@@ -1949,7 +1989,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2">
         <v>16.909468341842899</v>
@@ -2000,7 +2040,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2">
         <v>6.4675871875030904</v>
@@ -2051,17 +2091,32 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
+      </c>
+      <c r="L22" s="17">
+        <f>11*11*36*36*10 + 11</f>
+        <v>1568171</v>
+      </c>
+      <c r="M22" s="17">
+        <v>53064</v>
+      </c>
+      <c r="N22" s="10">
+        <f>M22/L22</f>
+        <v>3.3838146477648164E-2</v>
+      </c>
+      <c r="O22" s="21">
+        <f>(100*(1-K22))/M22</f>
+        <v>1.8845168098899443E-3</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2257,7 +2312,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B32" s="14">
         <v>0.83941484694104995</v>
@@ -2293,7 +2348,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B33" s="14">
         <v>0.85005608141446998</v>

</xml_diff>

<commit_message>
More results chart tweaking
</commit_message>
<xml_diff>
--- a/reports/ReportData.xlsx
+++ b/reports/ReportData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t xml:space="preserve">Test Errors by Variable </t>
   </si>
@@ -105,9 +105,6 @@
     <t>Accuracy per Complexity</t>
   </si>
   <si>
-    <t>Non-regularized results</t>
-  </si>
-  <si>
     <t>VAR(10) trained on single cell</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>VAR(1) trained on single cell</t>
   </si>
   <si>
-    <t>Lasso-regularized Results</t>
-  </si>
-  <si>
     <t>VAR(10) trained on all cells</t>
   </si>
   <si>
@@ -139,6 +133,15 @@
   </si>
   <si>
     <t>LR trained on single cell, LASSO</t>
+  </si>
+  <si>
+    <t>Non-Regularized</t>
+  </si>
+  <si>
+    <t>Non-regularized</t>
+  </si>
+  <si>
+    <t>Lasso-Regularized</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -230,6 +233,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -281,35 +285,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1200"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Test</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>RMSE for Single</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Cell Models</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t> </a:t>
+              <a:rPr lang="en-US" sz="1200" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Test-Set RMSE for All Tested Models  </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -333,7 +315,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Non-regularized results</c:v>
+                  <c:v>Non-Regularized</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -510,9 +492,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$7:$A$10</c:f>
+              <c:f>(Sheet1!$A$7:$A$10,Sheet1!$A$19:$A$22)</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>LR trained on single cell</c:v>
                 </c:pt>
@@ -524,16 +506,28 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>VAR(10) trained on single cell</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>LR trained on all cells</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VAR(1) trained on all cells</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VAR(2) trained on all cells</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VAR(10) trained on all cells</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$7:$K$10</c:f>
+              <c:f>(Sheet1!$K$7:$K$10,Sheet1!$K$19:$K$22)</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.30045917336864481</c:v>
                 </c:pt>
@@ -542,6 +536,21 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.43202177095691729</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9074952849113549</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34000365242911068</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.022220598901061</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.3440734467738693</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.173499763125323</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,13 +565,43 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Lasso-regularized Results</c:v>
+                  <c:v>Lasso-Regularized</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.4280408542246297E-3"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.1142061281337047E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -573,9 +612,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$7:$A$10</c:f>
+              <c:f>(Sheet1!$A$7:$A$10,Sheet1!$A$19:$A$22)</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>LR trained on single cell</c:v>
                 </c:pt>
@@ -587,16 +626,28 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>VAR(10) trained on single cell</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>LR trained on all cells</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>VAR(1) trained on all cells</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>VAR(2) trained on all cells</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>VAR(10) trained on all cells</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$13:$K$16</c:f>
+              <c:f>(Sheet1!$K$13:$K$16,Sheet1!$K$25:$K$28)</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="1">
                   <c:v>0.38068372610043122</c:v>
                 </c:pt>
@@ -605,6 +656,15 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.24577347486789469</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.40696888442147017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.41160035409866158</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45371670725940599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -618,7 +678,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="78"/>
+        <c:overlap val="1"/>
         <c:axId val="42005632"/>
         <c:axId val="42007168"/>
       </c:barChart>
@@ -633,11 +694,11 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
-          <a:bodyPr rot="-1920000" vert="horz"/>
+          <a:bodyPr rot="-3000000" vert="horz" anchor="ctr" anchorCtr="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr b="0"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -716,468 +777,20 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Test</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>RMSE for Multi-Cell Models</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t> </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Non-regularized results</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="66000"/>
-                      <a:satMod val="160000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="44500"/>
-                      <a:satMod val="160000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="23500"/>
-                      <a:satMod val="160000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:gradFill>
-                  <a:gsLst>
-                    <a:gs pos="0">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="66000"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="50000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="44500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="100000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="23500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                  </a:gsLst>
-                  <a:lin ang="5400000" scaled="0"/>
-                </a:gradFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:gradFill>
-                  <a:gsLst>
-                    <a:gs pos="0">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="66000"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="50000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="44500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="100000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="23500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                  </a:gsLst>
-                  <a:lin ang="5400000" scaled="0"/>
-                </a:gradFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:gradFill>
-                  <a:gsLst>
-                    <a:gs pos="0">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="66000"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="50000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="44500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="100000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="23500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                  </a:gsLst>
-                  <a:lin ang="5400000" scaled="0"/>
-                </a:gradFill>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="10"/>
-              <c:spPr/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="1"/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$19:$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>LR trained on all cells</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>VAR(1) trained on all cells</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>VAR(2) trained on all cells</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>VAR(10) trained on all cells</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$K$19:$K$22</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.34000365242911068</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.022220598901061</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.3440734467738693</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Lasso-regularized Results</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$19:$A$22</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>LR trained on all cells</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>VAR(1) trained on all cells</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>VAR(2) trained on all cells</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>VAR(10) trained on all cells</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$K$25:$K$28</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="1">
-                  <c:v>0.40696888442147017</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.41160035409866158</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.45371670725940599</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="105421824"/>
-        <c:axId val="108124800"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="105421824"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr rot="-1920000" vert="horz"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="108124800"/>
-        <c:crossesAt val="1.0000000000000002E-2"/>
-        <c:auto val="0"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="108124800"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-          <c:max val="100"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Error</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="out"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105421824"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
-        <c:minorUnit val="10"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>847725</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1352550</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1191,38 +804,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1752600</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1521,7 +1102,7 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,7 +1128,7 @@
       <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="11">
+      <c r="D1" s="12">
         <f>24*30*11*(6*6)</f>
         <v>285120</v>
       </c>
@@ -1594,10 +1175,10 @@
       <c r="K3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="12" t="s">
         <v>24</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -1609,62 +1190,62 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="15">
+      <c r="A7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="16">
         <v>0.66499208370129603</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="16">
         <v>0.22462674951502701</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="16">
         <v>0.62013620691839899</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="16">
         <v>0.26187400599183802</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="16">
         <v>0.25399311515710199</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="16">
         <v>0.28476794188613003</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="16">
         <v>9.6685907541825294E-2</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="16">
         <v>0.16891624611528699</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="16">
         <v>0.128140303490899</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="16">
         <f>AVERAGE(B7:J7)</f>
         <v>0.30045917336864481</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="23">
         <v>11</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="23">
         <v>11</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="16">
         <f>M7/L7</f>
         <v>1</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="24">
         <f>(100*(1-K7))/M7</f>
         <v>6.3594620602850478</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2">
         <v>0.95244427414566502</v>
@@ -1697,25 +1278,25 @@
         <f>AVERAGE(B8:J8)</f>
         <v>0.41973765135113006</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="19">
         <f>11*11 + 11</f>
         <v>132</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="19">
         <v>132</v>
       </c>
       <c r="N8" s="2">
         <f>M8/L8</f>
         <v>1</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="20">
         <f>(100*(1-K8))/M8</f>
         <v>0.43959268837035603</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2">
         <v>1.2007853203182199</v>
@@ -1748,35 +1329,80 @@
         <f>AVERAGE(B9:J9)</f>
         <v>0.43202177095691729</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="19">
         <f>11*11*2 + 11</f>
         <v>253</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="19">
         <v>253</v>
       </c>
       <c r="N9" s="2">
         <f>M9/L9</f>
         <v>1</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="20">
         <f>(100*(1-K9))/M9</f>
         <v>0.22449732373244374</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="11">
+        <v>4.8199210147203901</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2.2974842316423798</v>
+      </c>
+      <c r="D10" s="11">
+        <v>4.02368905499047</v>
+      </c>
+      <c r="E10" s="11">
+        <v>2.04209898984579</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.62747398337008298</v>
+      </c>
+      <c r="G10" s="11">
+        <v>1.06441324297629</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0.44280015759867802</v>
+      </c>
+      <c r="I10" s="11">
+        <v>1.46149192838258</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0.38808496067553599</v>
+      </c>
+      <c r="K10" s="11">
+        <f>AVERAGE(B10:J10)</f>
+        <v>1.9074952849113549</v>
+      </c>
+      <c r="L10" s="10">
+        <v>1221</v>
+      </c>
+      <c r="M10" s="10">
+        <v>1221</v>
+      </c>
+      <c r="N10" s="2">
+        <f>M10/L10</f>
+        <v>1</v>
+      </c>
+      <c r="O10" s="20">
+        <f>(100*(1-K10))/M10</f>
+        <v>-7.4323938158178129E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>40</v>
+      <c r="A13" s="14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1814,18 +1440,18 @@
         <f>AVERAGE(B14:J14)</f>
         <v>0.38068372610043122</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L14" s="17">
         <f>11*11 + 11</f>
         <v>132</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="17">
         <v>44</v>
       </c>
       <c r="N14" s="3">
         <f>M14/L14</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="O14" s="20">
+      <c r="O14" s="21">
         <f>(100*(1-K14))/M14</f>
         <v>1.4075369861353837</v>
       </c>
@@ -1865,18 +1491,18 @@
         <f>AVERAGE(B15:J15)</f>
         <v>0.38687578839041625</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="17">
         <f>11*11*2 + 11</f>
         <v>253</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="17">
         <v>51</v>
       </c>
       <c r="N15" s="3">
         <f>M15/L15</f>
         <v>0.20158102766798419</v>
       </c>
-      <c r="O15" s="20">
+      <c r="O15" s="21">
         <f>(100*(1-K15))/M15</f>
         <v>1.2022043364893797</v>
       </c>
@@ -1885,111 +1511,111 @@
       <c r="A16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="11">
         <v>0.30210303123493398</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="11">
         <v>0.13506319458712601</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="11">
         <v>0.36069485846007299</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="11">
         <v>0.32443797502070099</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="11">
         <v>0.25598129231854999</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="11">
         <v>0.288416432542352</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="11">
         <v>0.16975756166544401</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="11">
         <v>0.16991211370152801</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="11">
         <v>0.20559481428034401</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="11">
         <f>AVERAGE(B16:J16)</f>
         <v>0.24577347486789469</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="18">
         <f>11*11*10 + 11</f>
         <v>1221</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16" s="18">
         <v>81</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="11">
         <f>M16/L16</f>
         <v>6.6339066339066333E-2</v>
       </c>
-      <c r="O16" s="21">
+      <c r="O16" s="22">
         <f>(100*(1-K16))/M16</f>
         <v>0.93114385818778445</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="15">
+      <c r="A19" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="16">
         <v>0.89801268782257704</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="16">
         <v>0.22355063479144899</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="16">
         <v>0.72599486519848599</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="16">
         <v>0.28147514672004997</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="16">
         <v>0.24772788832555001</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="16">
         <v>0.29109880076323702</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="16">
         <v>8.5419443198951395E-2</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="16">
         <v>0.18107963513463801</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="16">
         <v>0.125673769907058</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K19" s="16">
         <f>AVERAGE(B19:J19)</f>
         <v>0.34000365242911068</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="23">
         <v>11</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="23">
         <v>11</v>
       </c>
-      <c r="N19" s="15">
+      <c r="N19" s="16">
         <f>M19/L19</f>
         <v>1</v>
       </c>
-      <c r="O19" s="23">
+      <c r="O19" s="24">
         <f>(100*(1-K19))/M19</f>
         <v>5.9999667960989935</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2">
         <v>16.909468341842899</v>
@@ -2022,25 +1648,25 @@
         <f>AVERAGE(B20:J20)</f>
         <v>18.022220598901061</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="19">
         <f>11*11*36*36 + 11</f>
         <v>156827</v>
       </c>
-      <c r="M20" s="18">
+      <c r="M20" s="19">
         <v>56628</v>
       </c>
       <c r="N20" s="2">
         <f>M20/L20</f>
         <v>0.36108578242266959</v>
       </c>
-      <c r="O20" s="19">
+      <c r="O20" s="20">
         <f>(100*(1-K20))/M20</f>
         <v>-3.0059724162783536E-2</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2">
         <v>6.4675871875030904</v>
@@ -2073,50 +1699,81 @@
         <f>AVERAGE(B21:J21)</f>
         <v>8.3440734467738693</v>
       </c>
-      <c r="L21" s="18">
+      <c r="L21" s="19">
         <f>11*11*36*36*2 + 11</f>
         <v>313643</v>
       </c>
-      <c r="M21" s="18">
+      <c r="M21" s="19">
         <v>56232</v>
       </c>
       <c r="N21" s="2">
         <f>M21/L21</f>
         <v>0.17928664118121559</v>
       </c>
-      <c r="O21" s="19">
+      <c r="O21" s="20">
         <f>(100*(1-K21))/M21</f>
         <v>-1.306030987120122E-2</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" s="17">
+        <v>32</v>
+      </c>
+      <c r="B22" s="11">
+        <v>3.0913751656416699</v>
+      </c>
+      <c r="C22" s="11">
+        <v>2.7321816920060198</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1.9479804852704801</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1.52861436386752</v>
+      </c>
+      <c r="F22" s="11">
+        <v>2.2905106684766299</v>
+      </c>
+      <c r="G22" s="11">
+        <v>2.6670258092713399</v>
+      </c>
+      <c r="H22" s="11">
+        <v>1.81526697518548</v>
+      </c>
+      <c r="I22" s="11">
+        <v>1.7102001056632701</v>
+      </c>
+      <c r="J22" s="11">
+        <v>1.7783426027455</v>
+      </c>
+      <c r="K22" s="11">
+        <f>AVERAGE(B22:J22)</f>
+        <v>2.173499763125323</v>
+      </c>
+      <c r="L22" s="18">
         <f>11*11*36*36*10 + 11</f>
         <v>1568171</v>
       </c>
-      <c r="M22" s="17">
+      <c r="M22" s="18">
         <v>53064</v>
       </c>
-      <c r="N22" s="10">
+      <c r="N22" s="11">
         <f>M22/L22</f>
         <v>3.3838146477648164E-2</v>
       </c>
-      <c r="O22" s="21">
+      <c r="O22" s="22">
         <f>(100*(1-K22))/M22</f>
-        <v>1.8845168098899443E-3</v>
+        <v>-2.2114800300115389E-3</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>39</v>
+      <c r="A25" s="14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2154,18 +1811,18 @@
         <f>AVERAGE(B26:J26)</f>
         <v>0.40696888442147017</v>
       </c>
-      <c r="L26" s="16">
+      <c r="L26" s="17">
         <f>11*11*36*36 + 11</f>
         <v>156827</v>
       </c>
-      <c r="M26" s="16">
+      <c r="M26" s="17">
         <v>3068</v>
       </c>
       <c r="N26" s="3">
         <f>M26/L26</f>
         <v>1.9562957909033521E-2</v>
       </c>
-      <c r="O26" s="20">
+      <c r="O26" s="21">
         <f>(100*(1-K26))/M26</f>
         <v>1.9329567000603971E-2</v>
       </c>
@@ -2205,18 +1862,18 @@
         <f>AVERAGE(B27:J27)</f>
         <v>0.41160035409866158</v>
       </c>
-      <c r="L27" s="16">
+      <c r="L27" s="17">
         <f>11*11*36*36*2 + 11</f>
         <v>313643</v>
       </c>
-      <c r="M27" s="16">
+      <c r="M27" s="17">
         <v>3559</v>
       </c>
       <c r="N27" s="3">
         <f>M27/L27</f>
         <v>1.1347296129676096E-2</v>
       </c>
-      <c r="O27" s="20">
+      <c r="O27" s="21">
         <f>(100*(1-K27))/M27</f>
         <v>1.6532723964634403E-2</v>
       </c>
@@ -2225,49 +1882,49 @@
       <c r="A28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="11">
         <v>1.17599775000313</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="11">
         <v>0.43086779871585601</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="11">
         <v>0.99431097428885895</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="11">
         <v>0.32627431090657599</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="11">
         <v>0.31716806888393301</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="11">
         <v>0.36637417322997901</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="11">
         <v>0.144640077764502</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="11">
         <v>0.124447814803434</v>
       </c>
-      <c r="J28" s="10">
+      <c r="J28" s="11">
         <v>0.203369396738386</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="11">
         <f>AVERAGE(B28:J28)</f>
         <v>0.45371670725940599</v>
       </c>
-      <c r="L28" s="17">
+      <c r="L28" s="18">
         <f>11*11*36*36*10 + 11</f>
         <v>1568171</v>
       </c>
-      <c r="M28" s="17">
+      <c r="M28" s="18">
         <v>5106</v>
       </c>
-      <c r="N28" s="10">
+      <c r="N28" s="11">
         <f>M28/L28</f>
         <v>3.2560224618361135E-3</v>
       </c>
-      <c r="O28" s="21">
+      <c r="O28" s="22">
         <f>(100*(1-K28))/M28</f>
         <v>1.0698850229937211E-2</v>
       </c>
@@ -2311,73 +1968,73 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="14">
+      <c r="A32" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="15">
         <v>0.83941484694104995</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="15">
         <v>0.225045197531864</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="15">
         <v>0.68864963765631904</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="15">
         <v>0.284679930064973</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="15">
         <v>0.248651136634783</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="15">
         <v>0.29152019723342798</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="15">
         <v>9.8795716452450402E-2</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I32" s="15">
         <v>0.180836089289061</v>
       </c>
-      <c r="J32" s="14">
+      <c r="J32" s="15">
         <v>0.12917784082234901</v>
       </c>
-      <c r="K32" s="15">
+      <c r="K32" s="16">
         <f>AVERAGE(B32:J32)</f>
         <v>0.3318633991806974</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="14">
+      <c r="A33" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="15">
         <v>0.85005608141446998</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="15">
         <v>0.221417217572243</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="15">
         <v>0.72505758090471795</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="15">
         <v>0.28736444954294699</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="15">
         <v>0.24964144326641599</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="15">
         <v>0.29400741346054399</v>
       </c>
-      <c r="H33" s="14">
+      <c r="H33" s="15">
         <v>8.5867325264773101E-2</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I33" s="15">
         <v>0.180381886448784</v>
       </c>
-      <c r="J33" s="14">
+      <c r="J33" s="15">
         <v>0.12588730187800101</v>
       </c>
-      <c r="K33" s="15">
+      <c r="K33" s="16">
         <f>AVERAGE(B33:J33)</f>
         <v>0.33552007775032178</v>
       </c>
@@ -2674,34 +2331,34 @@
       <c r="A42" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="13">
         <v>0.55126339908849697</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="13">
         <v>0.23466554908401899</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42" s="13">
         <v>0.42440352986424301</v>
       </c>
-      <c r="E42" s="12">
+      <c r="E42" s="13">
         <v>0.343155487594825</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F42" s="13">
         <v>0.25232636762174199</v>
       </c>
-      <c r="G42" s="12">
+      <c r="G42" s="13">
         <v>0.29383647862395601</v>
       </c>
-      <c r="H42" s="12">
+      <c r="H42" s="13">
         <v>0.17452330883971101</v>
       </c>
-      <c r="I42" s="12">
+      <c r="I42" s="13">
         <v>0.179401073826123</v>
       </c>
-      <c r="J42" s="12">
+      <c r="J42" s="13">
         <v>0.22804504622082</v>
       </c>
-      <c r="K42" s="10">
+      <c r="K42" s="11">
         <f>AVERAGE(B42:J42)</f>
         <v>0.29795780452932624</v>
       </c>
@@ -2710,34 +2367,34 @@
       <c r="A43" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B43" s="13">
         <v>0.30210303123493398</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="13">
         <v>0.13506319458712601</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="13">
         <v>0.36069485846007299</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E43" s="13">
         <v>0.32443797502070099</v>
       </c>
-      <c r="F43" s="12">
+      <c r="F43" s="13">
         <v>0.25598129231854999</v>
       </c>
-      <c r="G43" s="12">
+      <c r="G43" s="13">
         <v>0.288416432542352</v>
       </c>
-      <c r="H43" s="12">
+      <c r="H43" s="13">
         <v>0.16975756166544401</v>
       </c>
-      <c r="I43" s="12">
+      <c r="I43" s="13">
         <v>0.16991211370152801</v>
       </c>
-      <c r="J43" s="12">
+      <c r="J43" s="13">
         <v>0.20559481428034401</v>
       </c>
-      <c r="K43" s="10">
+      <c r="K43" s="11">
         <f>AVERAGE(B43:J43)</f>
         <v>0.24577347486789469</v>
       </c>

</xml_diff>

<commit_message>
Bit of report data
</commit_message>
<xml_diff>
--- a/reports/ReportData.xlsx
+++ b/reports/ReportData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19155" windowHeight="11310"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="19155" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t xml:space="preserve">Test Errors by Variable </t>
   </si>
@@ -129,12 +129,6 @@
     <t>LR trained on single cell</t>
   </si>
   <si>
-    <t>LR trained on all cells, LASSO</t>
-  </si>
-  <si>
-    <t>LR trained on single cell, LASSO</t>
-  </si>
-  <si>
     <t>Non-Regularized</t>
   </si>
   <si>
@@ -142,6 +136,18 @@
   </si>
   <si>
     <t>Lasso-Regularized</t>
+  </si>
+  <si>
+    <t>Baseline LR trained on single cell</t>
+  </si>
+  <si>
+    <t>Baseline LR trained on single cell, LASSO</t>
+  </si>
+  <si>
+    <t>Baseline LR trained on all cells</t>
+  </si>
+  <si>
+    <t>Baseline LR trained on all cells, LASSO</t>
   </si>
 </sst>
 </file>
@@ -150,7 +156,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -235,18 +241,18 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -288,10 +294,16 @@
               <a:defRPr sz="1200"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1200" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Test-Set RMSE for All Tested Models  </a:t>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Test</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Set RMSE for All Tested Models  </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -322,29 +334,9 @@
           </c:tx>
           <c:spPr>
             <a:ln>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="66000"/>
-                      <a:satMod val="160000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="44500"/>
-                      <a:satMod val="160000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="23500"/>
-                      <a:satMod val="160000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -354,35 +346,15 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent3">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
-                <a:gradFill>
-                  <a:gsLst>
-                    <a:gs pos="0">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="66000"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="50000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="44500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="100000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="23500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                  </a:gsLst>
-                  <a:lin ang="5400000" scaled="0"/>
-                </a:gradFill>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -391,36 +363,28 @@
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent3">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
-                <a:gradFill>
-                  <a:gsLst>
-                    <a:gs pos="0">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="66000"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="50000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="44500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="100000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="23500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                  </a:gsLst>
-                  <a:lin ang="5400000" scaled="0"/>
-                </a:gradFill>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
               </a:ln>
             </c:spPr>
           </c:dPt>
@@ -435,53 +399,13 @@
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
-                <a:gradFill>
-                  <a:gsLst>
-                    <a:gs pos="0">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="66000"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="50000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="44500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                    <a:gs pos="100000">
-                      <a:schemeClr val="accent1">
-                        <a:tint val="23500"/>
-                        <a:satMod val="160000"/>
-                      </a:schemeClr>
-                    </a:gs>
-                  </a:gsLst>
-                  <a:lin ang="5400000" scaled="0"/>
-                </a:gradFill>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="10"/>
-              <c:spPr/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="1"/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -496,7 +420,7 @@
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>LR trained on single cell</c:v>
+                  <c:v>Baseline LR trained on single cell</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>VAR(1) trained on single cell</c:v>
@@ -508,7 +432,7 @@
                   <c:v>VAR(10) trained on single cell</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LR trained on all cells</c:v>
+                  <c:v>Baseline LR trained on all cells</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>VAR(1) trained on all cells</c:v>
@@ -529,10 +453,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.30045917336864481</c:v>
+                  <c:v>0.33186339918069774</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41973765135113006</c:v>
+                  <c:v>0.34669746186640316</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.43202177095691729</c:v>
@@ -570,6 +494,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
@@ -616,7 +547,7 @@
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>LR trained on single cell</c:v>
+                  <c:v>Baseline LR trained on single cell</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>VAR(1) trained on single cell</c:v>
@@ -628,7 +559,7 @@
                   <c:v>VAR(10) trained on single cell</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LR trained on all cells</c:v>
+                  <c:v>Baseline LR trained on all cells</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>VAR(1) trained on all cells</c:v>
@@ -655,7 +586,7 @@
                   <c:v>0.38687578839041625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24577347486789469</c:v>
+                  <c:v>0.46139471824985506</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.40696888442147017</c:v>
@@ -680,11 +611,11 @@
         </c:dLbls>
         <c:gapWidth val="78"/>
         <c:overlap val="1"/>
-        <c:axId val="42005632"/>
-        <c:axId val="42007168"/>
+        <c:axId val="99725696"/>
+        <c:axId val="99727232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42005632"/>
+        <c:axId val="99725696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,16 +625,16 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
-          <a:bodyPr rot="-3000000" vert="horz" anchor="ctr" anchorCtr="0"/>
+          <a:bodyPr rot="-3000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0"/>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42007168"/>
+        <c:crossAx val="99727232"/>
         <c:crossesAt val="1.0000000000000002E-2"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -711,7 +642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42007168"/>
+        <c:axId val="99727232"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -743,7 +674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42005632"/>
+        <c:crossAx val="99725696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -759,7 +690,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr rtl="0">
-            <a:defRPr/>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -769,6 +703,399 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1" i="0" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Test Set RMSE by Meteorological Variable</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200">
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.5555555555555558E-3"/>
+                  <c:y val="9.2592592592592587E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.1111111111111112E-2"/>
+                  <c:y val="9.2592592592592587E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.5555555555555558E-3"/>
+                  <c:y val="1.3888888888888888E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.1111111111111059E-2"/>
+                  <c:y val="2.3148148148148147E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.3333333333333332E-3"/>
+                  <c:y val="1.3888888888888888E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.3333333333333332E-3"/>
+                  <c:y val="1.8518518518518517E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.5555555555555558E-3"/>
+                  <c:y val="1.3888888888888888E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0185067526415994E-16"/>
+                  <c:y val="-1.8518518518518517E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.3333333333333332E-3"/>
+                  <c:y val="-1.3888888888888846E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$3:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Precipitation</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Potential Energy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>% Convective</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>LW Radiation</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SW Radiation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Potential Evaporation</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Air Pressure</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Humidity</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Temperature</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.83941484694105095</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.225045197531864</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68864963765632004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.284679930064973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.248651136634784</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29152019723342798</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8795716452450597E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.18083608928906</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.12917784082234901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="88138112"/>
+        <c:axId val="88139648"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="88138112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88139648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88139648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88138112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -781,16 +1108,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>923925</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1352550</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -804,6 +1131,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1101,8 +1458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,49 +1547,49 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B7" s="16">
-        <v>0.66499208370129603</v>
+        <v>0.83941484694105095</v>
       </c>
       <c r="C7" s="16">
-        <v>0.22462674951502701</v>
+        <v>0.225045197531864</v>
       </c>
       <c r="D7" s="16">
-        <v>0.62013620691839899</v>
+        <v>0.68864963765632004</v>
       </c>
       <c r="E7" s="16">
-        <v>0.26187400599183802</v>
+        <v>0.284679930064973</v>
       </c>
       <c r="F7" s="16">
-        <v>0.25399311515710199</v>
+        <v>0.248651136634784</v>
       </c>
       <c r="G7" s="16">
-        <v>0.28476794188613003</v>
+        <v>0.29152019723342798</v>
       </c>
       <c r="H7" s="16">
-        <v>9.6685907541825294E-2</v>
+        <v>9.8795716452450597E-2</v>
       </c>
       <c r="I7" s="16">
-        <v>0.16891624611528699</v>
+        <v>0.18083608928906</v>
       </c>
       <c r="J7" s="16">
-        <v>0.128140303490899</v>
+        <v>0.12917784082234901</v>
       </c>
       <c r="K7" s="16">
         <f>AVERAGE(B7:J7)</f>
-        <v>0.30045917336864481</v>
+        <v>0.33186339918069774</v>
       </c>
       <c r="L7" s="23">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="M7" s="23">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="N7" s="16">
         <f>M7/L7</f>
@@ -1240,7 +1597,7 @@
       </c>
       <c r="O7" s="24">
         <f>(100*(1-K7))/M7</f>
-        <v>6.3594620602850478</v>
+        <v>0.50616409152977437</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1248,35 +1605,35 @@
         <v>31</v>
       </c>
       <c r="B8" s="2">
-        <v>0.95244427414566502</v>
+        <v>0.78703640727055002</v>
       </c>
       <c r="C8" s="2">
-        <v>0.267223846753677</v>
+        <v>0.20716210698228801</v>
       </c>
       <c r="D8" s="2">
-        <v>1.0634252955158401</v>
+        <v>0.72547259024084698</v>
       </c>
       <c r="E8" s="2">
-        <v>0.32332556043647598</v>
+        <v>0.33927462277570603</v>
       </c>
       <c r="F8" s="2">
-        <v>0.33284930089528297</v>
+        <v>0.25890629063702197</v>
       </c>
       <c r="G8" s="2">
-        <v>0.37780950287765502</v>
+        <v>0.421854868954472</v>
       </c>
       <c r="H8" s="2">
-        <v>0.159083461202328</v>
+        <v>9.8730296724049704E-2</v>
       </c>
       <c r="I8" s="2">
-        <v>0.130244619625208</v>
+        <v>0.141635156925463</v>
       </c>
       <c r="J8" s="2">
-        <v>0.17123300070803801</v>
+        <v>0.140204816287231</v>
       </c>
       <c r="K8" s="2">
         <f>AVERAGE(B8:J8)</f>
-        <v>0.41973765135113006</v>
+        <v>0.34669746186640316</v>
       </c>
       <c r="L8" s="19">
         <f>11*11 + 11</f>
@@ -1291,7 +1648,7 @@
       </c>
       <c r="O8" s="20">
         <f>(100*(1-K8))/M8</f>
-        <v>0.43959268837035603</v>
+        <v>0.49492616525272493</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1397,12 +1754,12 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1512,35 +1869,35 @@
         <v>20</v>
       </c>
       <c r="B16" s="11">
-        <v>0.30210303123493398</v>
+        <v>1.3841026932149201</v>
       </c>
       <c r="C16" s="11">
-        <v>0.13506319458712601</v>
+        <v>0.31346945592012099</v>
       </c>
       <c r="D16" s="11">
-        <v>0.36069485846007299</v>
+        <v>0.92993356385043402</v>
       </c>
       <c r="E16" s="11">
-        <v>0.32443797502070099</v>
+        <v>0.317090661950087</v>
       </c>
       <c r="F16" s="11">
-        <v>0.25598129231854999</v>
+        <v>0.31597301681990902</v>
       </c>
       <c r="G16" s="11">
-        <v>0.288416432542352</v>
+        <v>0.39152690031303999</v>
       </c>
       <c r="H16" s="11">
-        <v>0.16975756166544401</v>
+        <v>0.13999332703178799</v>
       </c>
       <c r="I16" s="11">
-        <v>0.16991211370152801</v>
+        <v>0.117059647792616</v>
       </c>
       <c r="J16" s="11">
-        <v>0.20559481428034401</v>
+        <v>0.24340319735578</v>
       </c>
       <c r="K16" s="11">
         <f>AVERAGE(B16:J16)</f>
-        <v>0.24577347486789469</v>
+        <v>0.46139471824985506</v>
       </c>
       <c r="L16" s="18">
         <f>11*11*10 + 11</f>
@@ -1555,17 +1912,17 @@
       </c>
       <c r="O16" s="22">
         <f>(100*(1-K16))/M16</f>
-        <v>0.93114385818778445</v>
+        <v>0.66494479228412962</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B19" s="16">
         <v>0.89801268782257704</v>
@@ -1599,10 +1956,10 @@
         <v>0.34000365242911068</v>
       </c>
       <c r="L19" s="23">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="M19" s="23">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="N19" s="16">
         <f>M19/L19</f>
@@ -1610,7 +1967,7 @@
       </c>
       <c r="O19" s="24">
         <f>(100*(1-K19))/M19</f>
-        <v>5.9999667960989935</v>
+        <v>0.49999723300824944</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1768,12 +2125,12 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1972,35 +2329,35 @@
         <v>36</v>
       </c>
       <c r="B32" s="15">
-        <v>0.83941484694104995</v>
+        <v>0.83941484694105095</v>
       </c>
       <c r="C32" s="15">
         <v>0.225045197531864</v>
       </c>
       <c r="D32" s="15">
-        <v>0.68864963765631904</v>
+        <v>0.68864963765632004</v>
       </c>
       <c r="E32" s="15">
         <v>0.284679930064973</v>
       </c>
       <c r="F32" s="15">
-        <v>0.248651136634783</v>
+        <v>0.248651136634784</v>
       </c>
       <c r="G32" s="15">
         <v>0.29152019723342798</v>
       </c>
       <c r="H32" s="15">
-        <v>9.8795716452450402E-2</v>
+        <v>9.8795716452450597E-2</v>
       </c>
       <c r="I32" s="15">
-        <v>0.180836089289061</v>
+        <v>0.18083608928906</v>
       </c>
       <c r="J32" s="15">
         <v>0.12917784082234901</v>
       </c>
       <c r="K32" s="16">
-        <f>AVERAGE(B32:J32)</f>
-        <v>0.3318633991806974</v>
+        <f t="shared" ref="K32:K43" si="0">AVERAGE(B32:J32)</f>
+        <v>0.33186339918069774</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2035,7 +2392,7 @@
         <v>0.12588730187800101</v>
       </c>
       <c r="K33" s="16">
-        <f>AVERAGE(B33:J33)</f>
+        <f t="shared" si="0"/>
         <v>0.33552007775032178</v>
       </c>
     </row>
@@ -2071,7 +2428,7 @@
         <v>0.12953776267733599</v>
       </c>
       <c r="K34" s="2">
-        <f>AVERAGE(B34:J34)</f>
+        <f t="shared" si="0"/>
         <v>0.29844229772215991</v>
       </c>
     </row>
@@ -2107,7 +2464,7 @@
         <v>4.8408873829520103E-14</v>
       </c>
       <c r="K35" s="2">
-        <f>AVERAGE(B35:J35)</f>
+        <f t="shared" si="0"/>
         <v>1.8582883083022425E-13</v>
       </c>
     </row>
@@ -2143,7 +2500,7 @@
         <v>9.6914901147014496E-2</v>
       </c>
       <c r="K36" s="2">
-        <f>AVERAGE(B36:J36)</f>
+        <f t="shared" si="0"/>
         <v>0.2438963987735937</v>
       </c>
     </row>
@@ -2179,7 +2536,7 @@
         <v>2.5177647765364999E-14</v>
       </c>
       <c r="K37" s="2">
-        <f>AVERAGE(B37:J37)</f>
+        <f t="shared" si="0"/>
         <v>5.3604651393890388E-14</v>
       </c>
     </row>
@@ -2215,7 +2572,7 @@
         <v>0.22096438696447199</v>
       </c>
       <c r="K38" s="3">
-        <f>AVERAGE(B38:J38)</f>
+        <f t="shared" si="0"/>
         <v>0.34388126035176581</v>
       </c>
     </row>
@@ -2251,7 +2608,7 @@
         <v>0.19964930182079199</v>
       </c>
       <c r="K39" s="3">
-        <f>AVERAGE(B39:J39)</f>
+        <f t="shared" si="0"/>
         <v>0.30310816191980222</v>
       </c>
     </row>
@@ -2287,7 +2644,7 @@
         <v>0.22126225808487501</v>
       </c>
       <c r="K40" s="3">
-        <f>AVERAGE(B40:J40)</f>
+        <f t="shared" si="0"/>
         <v>0.33324033779980722</v>
       </c>
     </row>
@@ -2323,7 +2680,7 @@
         <v>0.19965831421357899</v>
       </c>
       <c r="K41" s="3">
-        <f>AVERAGE(B41:J41)</f>
+        <f t="shared" si="0"/>
         <v>0.2951241339632012</v>
       </c>
     </row>
@@ -2359,7 +2716,7 @@
         <v>0.22804504622082</v>
       </c>
       <c r="K42" s="11">
-        <f>AVERAGE(B42:J42)</f>
+        <f t="shared" si="0"/>
         <v>0.29795780452932624</v>
       </c>
     </row>
@@ -2395,7 +2752,7 @@
         <v>0.20559481428034401</v>
       </c>
       <c r="K43" s="11">
-        <f>AVERAGE(B43:J43)</f>
+        <f t="shared" si="0"/>
         <v>0.24577347486789469</v>
       </c>
     </row>

</xml_diff>